<commit_message>
Update diploma generator models
</commit_message>
<xml_diff>
--- a/src/dataset/diploma.xlsx
+++ b/src/dataset/diploma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Merdani_ITServices\Docs\repo\diploma_topic_generator\src\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B126CAF-1C40-499A-A265-EAAFA4580893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FFCC49-343F-46B0-852B-0110D1E7865E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="2565" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5250" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3314,10 +3314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E446"/>
+  <dimension ref="A1:E531"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A442" workbookViewId="0">
+      <selection activeCell="A440" sqref="A440"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10909,6 +10909,346 @@
         <v>736</v>
       </c>
     </row>
+    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D447"/>
+      <c r="E447"/>
+    </row>
+    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D448"/>
+      <c r="E448"/>
+    </row>
+    <row r="449" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D449"/>
+      <c r="E449"/>
+    </row>
+    <row r="450" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D450"/>
+      <c r="E450"/>
+    </row>
+    <row r="451" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D451"/>
+      <c r="E451"/>
+    </row>
+    <row r="452" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D452"/>
+      <c r="E452"/>
+    </row>
+    <row r="453" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D453"/>
+      <c r="E453"/>
+    </row>
+    <row r="454" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D454"/>
+      <c r="E454"/>
+    </row>
+    <row r="455" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D455"/>
+      <c r="E455"/>
+    </row>
+    <row r="456" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D456"/>
+      <c r="E456"/>
+    </row>
+    <row r="457" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D457"/>
+      <c r="E457"/>
+    </row>
+    <row r="458" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D458"/>
+      <c r="E458"/>
+    </row>
+    <row r="459" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D459"/>
+      <c r="E459"/>
+    </row>
+    <row r="460" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D460"/>
+      <c r="E460"/>
+    </row>
+    <row r="461" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D461"/>
+      <c r="E461"/>
+    </row>
+    <row r="462" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D462"/>
+      <c r="E462"/>
+    </row>
+    <row r="463" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D463"/>
+      <c r="E463"/>
+    </row>
+    <row r="464" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D464"/>
+      <c r="E464"/>
+    </row>
+    <row r="465" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D465"/>
+      <c r="E465"/>
+    </row>
+    <row r="466" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D466"/>
+      <c r="E466"/>
+    </row>
+    <row r="467" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D467"/>
+      <c r="E467"/>
+    </row>
+    <row r="468" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D468"/>
+      <c r="E468"/>
+    </row>
+    <row r="469" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D469"/>
+      <c r="E469"/>
+    </row>
+    <row r="470" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D470"/>
+      <c r="E470"/>
+    </row>
+    <row r="471" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D471"/>
+      <c r="E471"/>
+    </row>
+    <row r="472" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D472"/>
+      <c r="E472"/>
+    </row>
+    <row r="473" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D473"/>
+      <c r="E473"/>
+    </row>
+    <row r="474" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D474"/>
+      <c r="E474"/>
+    </row>
+    <row r="475" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D475"/>
+      <c r="E475"/>
+    </row>
+    <row r="476" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D476"/>
+      <c r="E476"/>
+    </row>
+    <row r="477" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D477"/>
+      <c r="E477"/>
+    </row>
+    <row r="478" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D478"/>
+      <c r="E478"/>
+    </row>
+    <row r="479" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D479"/>
+      <c r="E479"/>
+    </row>
+    <row r="480" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D480"/>
+      <c r="E480"/>
+    </row>
+    <row r="481" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D481"/>
+      <c r="E481"/>
+    </row>
+    <row r="482" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D482"/>
+      <c r="E482"/>
+    </row>
+    <row r="483" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D483"/>
+      <c r="E483"/>
+    </row>
+    <row r="484" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D484"/>
+      <c r="E484"/>
+    </row>
+    <row r="485" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D485"/>
+      <c r="E485"/>
+    </row>
+    <row r="486" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D486"/>
+      <c r="E486"/>
+    </row>
+    <row r="487" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D487"/>
+      <c r="E487"/>
+    </row>
+    <row r="488" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D488"/>
+      <c r="E488"/>
+    </row>
+    <row r="489" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D489"/>
+      <c r="E489"/>
+    </row>
+    <row r="490" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D490"/>
+      <c r="E490"/>
+    </row>
+    <row r="491" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D491"/>
+      <c r="E491"/>
+    </row>
+    <row r="492" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D492"/>
+      <c r="E492"/>
+    </row>
+    <row r="493" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D493"/>
+      <c r="E493"/>
+    </row>
+    <row r="494" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D494"/>
+      <c r="E494"/>
+    </row>
+    <row r="495" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D495"/>
+      <c r="E495"/>
+    </row>
+    <row r="496" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D496"/>
+      <c r="E496"/>
+    </row>
+    <row r="497" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D497"/>
+      <c r="E497"/>
+    </row>
+    <row r="498" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D498"/>
+      <c r="E498"/>
+    </row>
+    <row r="499" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D499"/>
+      <c r="E499"/>
+    </row>
+    <row r="500" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D500"/>
+      <c r="E500"/>
+    </row>
+    <row r="501" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D501"/>
+      <c r="E501"/>
+    </row>
+    <row r="502" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D502"/>
+      <c r="E502"/>
+    </row>
+    <row r="503" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D503"/>
+      <c r="E503"/>
+    </row>
+    <row r="504" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D504"/>
+      <c r="E504"/>
+    </row>
+    <row r="505" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D505"/>
+      <c r="E505"/>
+    </row>
+    <row r="506" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D506"/>
+      <c r="E506"/>
+    </row>
+    <row r="507" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D507"/>
+      <c r="E507"/>
+    </row>
+    <row r="508" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D508"/>
+      <c r="E508"/>
+    </row>
+    <row r="509" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D509"/>
+      <c r="E509"/>
+    </row>
+    <row r="510" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D510"/>
+      <c r="E510"/>
+    </row>
+    <row r="511" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D511"/>
+      <c r="E511"/>
+    </row>
+    <row r="512" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D512"/>
+      <c r="E512"/>
+    </row>
+    <row r="513" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D513"/>
+      <c r="E513"/>
+    </row>
+    <row r="514" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D514"/>
+      <c r="E514"/>
+    </row>
+    <row r="515" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D515"/>
+      <c r="E515"/>
+    </row>
+    <row r="516" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D516"/>
+      <c r="E516"/>
+    </row>
+    <row r="517" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D517"/>
+      <c r="E517"/>
+    </row>
+    <row r="518" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D518"/>
+      <c r="E518"/>
+    </row>
+    <row r="519" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D519"/>
+      <c r="E519"/>
+    </row>
+    <row r="520" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D520"/>
+      <c r="E520"/>
+    </row>
+    <row r="521" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D521"/>
+      <c r="E521"/>
+    </row>
+    <row r="522" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D522"/>
+      <c r="E522"/>
+    </row>
+    <row r="523" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D523"/>
+      <c r="E523"/>
+    </row>
+    <row r="524" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D524"/>
+      <c r="E524"/>
+    </row>
+    <row r="525" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D525"/>
+      <c r="E525"/>
+    </row>
+    <row r="526" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D526"/>
+      <c r="E526"/>
+    </row>
+    <row r="527" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D527"/>
+      <c r="E527"/>
+    </row>
+    <row r="528" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D528"/>
+      <c r="E528"/>
+    </row>
+    <row r="529" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D529"/>
+      <c r="E529"/>
+    </row>
+    <row r="530" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D530"/>
+      <c r="E530"/>
+    </row>
+    <row r="531" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D531"/>
+      <c r="E531"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>